<commit_message>
Actualización General Proyecto AthletIA + Documentación al día.
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Sprints/Burdown Chart/Burndown Chart – Sprint 2 (25–29 Agosto).xlsx
+++ b/Fase 2/Evidencias Proyecto/Sprints/Burdown Chart/Burndown Chart – Sprint 2 (25–29 Agosto).xlsx
@@ -316,11 +316,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="570384290"/>
-        <c:axId val="1675677039"/>
+        <c:axId val="1451725541"/>
+        <c:axId val="1928933345"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="570384290"/>
+        <c:axId val="1451725541"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,10 +372,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1675677039"/>
+        <c:crossAx val="1928933345"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1675677039"/>
+        <c:axId val="1928933345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,7 +450,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570384290"/>
+        <c:crossAx val="1451725541"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -735,7 +735,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" ht="22.5" customHeight="1">
       <c r="F6" s="2" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="22.5" customHeight="1">
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
@@ -776,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="22.5" customHeight="1">
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
@@ -797,7 +797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="22.5" customHeight="1">
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
@@ -818,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="22.5" customHeight="1">
       <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
@@ -839,7 +839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="22.5" customHeight="1">
       <c r="F11" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>